<commit_message>
atualização ano base 2023
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2023/consumidores_a.xlsx
+++ b/inst/dados_premissas/2023/consumidores_a.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -413,11 +413,6 @@
           <t>2022</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -455,9 +450,6 @@
       <c r="K2">
         <v>2767</v>
       </c>
-      <c r="L2">
-        <v>2767</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -495,9 +487,6 @@
       <c r="K3">
         <v>652</v>
       </c>
-      <c r="L3">
-        <v>644</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -535,9 +524,6 @@
       <c r="K4">
         <v>2398</v>
       </c>
-      <c r="L4">
-        <v>2501</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -575,9 +561,6 @@
       <c r="K5">
         <v>4546</v>
       </c>
-      <c r="L5">
-        <v>4172</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -615,9 +598,6 @@
       <c r="K6">
         <v>10202</v>
       </c>
-      <c r="L6">
-        <v>10376</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -655,9 +635,6 @@
       <c r="K7">
         <v>5518</v>
       </c>
-      <c r="L7">
-        <v>5472</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -695,9 +672,6 @@
       <c r="K8">
         <v>13614</v>
       </c>
-      <c r="L8">
-        <v>13571</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -735,9 +709,6 @@
       <c r="K9">
         <v>83</v>
       </c>
-      <c r="L9">
-        <v>83</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -775,9 +746,6 @@
       <c r="K10">
         <v>183</v>
       </c>
-      <c r="L10">
-        <v>179</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -815,9 +783,6 @@
       <c r="K11">
         <v>8163</v>
       </c>
-      <c r="L11">
-        <v>7945</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -855,9 +820,6 @@
       <c r="K12">
         <v>96</v>
       </c>
-      <c r="L12">
-        <v>98</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -895,9 +857,6 @@
       <c r="K13">
         <v>13149</v>
       </c>
-      <c r="L13">
-        <v>13236</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -935,9 +894,6 @@
       <c r="K14">
         <v>2483</v>
       </c>
-      <c r="L14">
-        <v>2812</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -975,9 +931,6 @@
       <c r="K15">
         <v>14336</v>
       </c>
-      <c r="L15">
-        <v>12628</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1015,9 +968,6 @@
       <c r="K16">
         <v>4743</v>
       </c>
-      <c r="L16">
-        <v>4730</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1055,9 +1005,6 @@
       <c r="K17">
         <v>1548</v>
       </c>
-      <c r="L17">
-        <v>1553</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1095,9 +1042,6 @@
       <c r="K18">
         <v>158</v>
       </c>
-      <c r="L18">
-        <v>105</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1135,9 +1079,6 @@
       <c r="K19">
         <v>80</v>
       </c>
-      <c r="L19">
-        <v>75</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1175,9 +1116,6 @@
       <c r="K20">
         <v>158</v>
       </c>
-      <c r="L20">
-        <v>153</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1215,9 +1153,6 @@
       <c r="K21">
         <v>753</v>
       </c>
-      <c r="L21">
-        <v>760</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1292,9 +1227,6 @@
       <c r="K23">
         <v>2816</v>
       </c>
-      <c r="L23">
-        <v>2990</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1332,9 +1264,6 @@
       <c r="K24">
         <v>3732</v>
       </c>
-      <c r="L24">
-        <v>3645</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1372,9 +1301,6 @@
       <c r="K25">
         <v>8</v>
       </c>
-      <c r="L25">
-        <v>6</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1412,9 +1338,6 @@
       <c r="K26">
         <v>20</v>
       </c>
-      <c r="L26">
-        <v>19</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1452,9 +1375,6 @@
       <c r="K27">
         <v>6365</v>
       </c>
-      <c r="L27">
-        <v>6235</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1492,9 +1412,6 @@
       <c r="K28">
         <v>135</v>
       </c>
-      <c r="L28">
-        <v>104</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1532,9 +1449,6 @@
       <c r="K29">
         <v>189</v>
       </c>
-      <c r="L29">
-        <v>167</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1603,9 +1517,6 @@
       <c r="K31">
         <v>3039</v>
       </c>
-      <c r="L31">
-        <v>3193</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1643,9 +1554,6 @@
       <c r="K32">
         <v>5448</v>
       </c>
-      <c r="L32">
-        <v>6128</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1683,9 +1591,6 @@
       <c r="K33">
         <v>9761</v>
       </c>
-      <c r="L33">
-        <v>8205</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1723,9 +1628,6 @@
       <c r="K34">
         <v>5547</v>
       </c>
-      <c r="L34">
-        <v>4548</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1763,9 +1665,6 @@
       <c r="K35">
         <v>10895</v>
       </c>
-      <c r="L35">
-        <v>10194</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1840,9 +1739,6 @@
       <c r="K37">
         <v>1748</v>
       </c>
-      <c r="L37">
-        <v>2404</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1880,9 +1776,6 @@
       <c r="K38">
         <v>2157</v>
       </c>
-      <c r="L38">
-        <v>2185</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1920,9 +1813,6 @@
       <c r="K39">
         <v>7950</v>
       </c>
-      <c r="L39">
-        <v>7934</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1960,9 +1850,6 @@
       <c r="K40">
         <v>3001</v>
       </c>
-      <c r="L40">
-        <v>3052</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2000,9 +1887,6 @@
       <c r="K41">
         <v>4400</v>
       </c>
-      <c r="L41">
-        <v>4392</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2040,9 +1924,6 @@
       <c r="K42">
         <v>1926</v>
       </c>
-      <c r="L42">
-        <v>1977</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2080,9 +1961,6 @@
       <c r="K43">
         <v>2219</v>
       </c>
-      <c r="L43">
-        <v>2257</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2120,9 +1998,6 @@
       <c r="K44">
         <v>1172</v>
       </c>
-      <c r="L44">
-        <v>1148</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2160,9 +2035,6 @@
       <c r="K45">
         <v>1957</v>
       </c>
-      <c r="L45">
-        <v>1936</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2200,9 +2072,6 @@
       <c r="K46">
         <v>1268</v>
       </c>
-      <c r="L46">
-        <v>1266</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2240,9 +2109,6 @@
       <c r="K47">
         <v>74</v>
       </c>
-      <c r="L47">
-        <v>77</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2280,9 +2146,6 @@
       <c r="K48">
         <v>4646</v>
       </c>
-      <c r="L48">
-        <v>4421</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2320,9 +2183,6 @@
       <c r="K49">
         <v>27</v>
       </c>
-      <c r="L49">
-        <v>26</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2360,9 +2220,6 @@
       <c r="K50">
         <v>2967</v>
       </c>
-      <c r="L50">
-        <v>3073</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2400,9 +2257,6 @@
       <c r="K51">
         <v>22</v>
       </c>
-      <c r="L51">
-        <v>25</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2440,9 +2294,6 @@
       <c r="K52">
         <v>11259</v>
       </c>
-      <c r="L52">
-        <v>9751</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2480,9 +2331,6 @@
       <c r="K53">
         <v>820</v>
       </c>
-      <c r="L53">
-        <v>866</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2520,9 +2368,6 @@
       <c r="K54">
         <v>111</v>
       </c>
-      <c r="L54">
-        <v>113</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2559,9 +2404,6 @@
       </c>
       <c r="K55">
         <v>49</v>
-      </c>
-      <c r="L55">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrupamento de distribuidoras ENF+EMG=EMR e EBO+EPB=EPB
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2023/consumidores_a.xlsx
+++ b/inst/dados_premissas/2023/consumidores_a.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -413,6 +413,11 @@
           <t>2022</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -450,6 +455,9 @@
       <c r="K2">
         <v>2767</v>
       </c>
+      <c r="L2">
+        <v>2760</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -487,6 +495,9 @@
       <c r="K3">
         <v>652</v>
       </c>
+      <c r="L3">
+        <v>640</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -524,6 +535,9 @@
       <c r="K4">
         <v>2398</v>
       </c>
+      <c r="L4">
+        <v>2508</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -561,6 +575,9 @@
       <c r="K5">
         <v>4546</v>
       </c>
+      <c r="L5">
+        <v>4270</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -598,6 +615,9 @@
       <c r="K6">
         <v>10202</v>
       </c>
+      <c r="L6">
+        <v>10374</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -635,6 +655,9 @@
       <c r="K7">
         <v>5518</v>
       </c>
+      <c r="L7">
+        <v>5494</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -672,6 +695,9 @@
       <c r="K8">
         <v>13614</v>
       </c>
+      <c r="L8">
+        <v>13431</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -709,6 +735,9 @@
       <c r="K9">
         <v>83</v>
       </c>
+      <c r="L9">
+        <v>83</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -746,6 +775,9 @@
       <c r="K10">
         <v>183</v>
       </c>
+      <c r="L10">
+        <v>179</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -783,6 +815,9 @@
       <c r="K11">
         <v>8163</v>
       </c>
+      <c r="L11">
+        <v>7946</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -820,6 +855,9 @@
       <c r="K12">
         <v>96</v>
       </c>
+      <c r="L12">
+        <v>97</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -857,6 +895,9 @@
       <c r="K13">
         <v>13149</v>
       </c>
+      <c r="L13">
+        <v>13242</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -894,6 +935,9 @@
       <c r="K14">
         <v>2483</v>
       </c>
+      <c r="L14">
+        <v>2837</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -931,6 +975,9 @@
       <c r="K15">
         <v>14336</v>
       </c>
+      <c r="L15">
+        <v>16635</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -968,6 +1015,9 @@
       <c r="K16">
         <v>4743</v>
       </c>
+      <c r="L16">
+        <v>5205</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1005,6 +1055,9 @@
       <c r="K17">
         <v>1548</v>
       </c>
+      <c r="L17">
+        <v>1666</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1042,6 +1095,9 @@
       <c r="K18">
         <v>158</v>
       </c>
+      <c r="L18">
+        <v>105</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1079,6 +1135,9 @@
       <c r="K19">
         <v>80</v>
       </c>
+      <c r="L19">
+        <v>76</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1116,6 +1175,9 @@
       <c r="K20">
         <v>158</v>
       </c>
+      <c r="L20">
+        <v>154</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1153,1257 +1215,1288 @@
       <c r="K21">
         <v>753</v>
       </c>
+      <c r="L21">
+        <v>765</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>EBO</t>
+          <t>EDP ES</t>
         </is>
       </c>
       <c r="B22">
-        <v>342</v>
+        <v>3199</v>
       </c>
       <c r="C22">
-        <v>361</v>
+        <v>3375</v>
       </c>
       <c r="D22">
-        <v>375</v>
+        <v>3396</v>
       </c>
       <c r="E22">
-        <v>375</v>
+        <v>3257</v>
       </c>
       <c r="F22">
-        <v>373</v>
+        <v>3167</v>
       </c>
       <c r="G22">
-        <v>385</v>
+        <v>3125</v>
       </c>
       <c r="H22">
-        <v>389</v>
+        <v>3068</v>
       </c>
       <c r="I22">
-        <v>360</v>
+        <v>2995</v>
       </c>
       <c r="J22">
-        <v>364</v>
+        <v>2964</v>
       </c>
       <c r="K22">
-        <v>362</v>
+        <v>2816</v>
+      </c>
+      <c r="L22">
+        <v>2895</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>EDP ES</t>
+          <t>EDP SP</t>
         </is>
       </c>
       <c r="B23">
-        <v>3199</v>
+        <v>4078</v>
       </c>
       <c r="C23">
-        <v>3375</v>
+        <v>4174</v>
       </c>
       <c r="D23">
-        <v>3396</v>
+        <v>3950</v>
       </c>
       <c r="E23">
-        <v>3257</v>
+        <v>4079</v>
       </c>
       <c r="F23">
-        <v>3167</v>
+        <v>4589</v>
       </c>
       <c r="G23">
-        <v>3125</v>
+        <v>4129</v>
       </c>
       <c r="H23">
-        <v>3068</v>
+        <v>3598</v>
       </c>
       <c r="I23">
-        <v>2995</v>
+        <v>4016</v>
       </c>
       <c r="J23">
-        <v>2964</v>
+        <v>3757</v>
       </c>
       <c r="K23">
-        <v>2816</v>
+        <v>3732</v>
+      </c>
+      <c r="L23">
+        <v>3645</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>EDP SP</t>
+          <t>EFLJC</t>
         </is>
       </c>
       <c r="B24">
-        <v>4078</v>
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>4174</v>
+        <v>13</v>
       </c>
       <c r="D24">
-        <v>3950</v>
+        <v>12</v>
       </c>
       <c r="E24">
-        <v>4079</v>
+        <v>9</v>
       </c>
       <c r="F24">
-        <v>4589</v>
+        <v>7</v>
       </c>
       <c r="G24">
-        <v>4129</v>
+        <v>7</v>
       </c>
       <c r="H24">
-        <v>3598</v>
+        <v>7</v>
       </c>
       <c r="I24">
-        <v>4016</v>
+        <v>8</v>
       </c>
       <c r="J24">
-        <v>3757</v>
+        <v>7</v>
       </c>
       <c r="K24">
-        <v>3732</v>
+        <v>8</v>
+      </c>
+      <c r="L24">
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>EFLJC</t>
+          <t>EFLUL</t>
         </is>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C25">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D25">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E25">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="G25">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="H25">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="I25">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J25">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="K25">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="L25">
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>EFLUL</t>
+          <t>ELEKTRO</t>
         </is>
       </c>
       <c r="B26">
-        <v>34</v>
+        <v>6774</v>
       </c>
       <c r="C26">
-        <v>36</v>
+        <v>6944</v>
       </c>
       <c r="D26">
-        <v>35</v>
+        <v>7041</v>
       </c>
       <c r="E26">
-        <v>29</v>
+        <v>6811</v>
       </c>
       <c r="F26">
-        <v>30</v>
+        <v>6749</v>
       </c>
       <c r="G26">
-        <v>28</v>
+        <v>6772</v>
       </c>
       <c r="H26">
-        <v>28</v>
+        <v>6626</v>
       </c>
       <c r="I26">
-        <v>20</v>
+        <v>6509</v>
       </c>
       <c r="J26">
-        <v>21</v>
+        <v>6371</v>
       </c>
       <c r="K26">
-        <v>20</v>
+        <v>6365</v>
+      </c>
+      <c r="L26">
+        <v>6296</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ELEKTRO</t>
+          <t>ELETROCAR</t>
         </is>
       </c>
       <c r="B27">
-        <v>6774</v>
+        <v>118</v>
       </c>
       <c r="C27">
-        <v>6944</v>
+        <v>130</v>
       </c>
       <c r="D27">
-        <v>7041</v>
+        <v>141</v>
       </c>
       <c r="E27">
-        <v>6811</v>
+        <v>147</v>
       </c>
       <c r="F27">
-        <v>6749</v>
+        <v>146</v>
       </c>
       <c r="G27">
-        <v>6772</v>
+        <v>144</v>
       </c>
       <c r="H27">
-        <v>6626</v>
+        <v>134</v>
       </c>
       <c r="I27">
-        <v>6509</v>
+        <v>130</v>
       </c>
       <c r="J27">
-        <v>6371</v>
+        <v>126</v>
       </c>
       <c r="K27">
-        <v>6365</v>
+        <v>135</v>
+      </c>
+      <c r="L27">
+        <v>112</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ELETROCAR</t>
+          <t>ELFSM</t>
         </is>
       </c>
       <c r="B28">
-        <v>118</v>
+        <v>213</v>
       </c>
       <c r="C28">
-        <v>130</v>
+        <v>227</v>
       </c>
       <c r="D28">
-        <v>141</v>
+        <v>230</v>
       </c>
       <c r="E28">
-        <v>147</v>
+        <v>228</v>
       </c>
       <c r="F28">
-        <v>146</v>
+        <v>221</v>
       </c>
       <c r="G28">
-        <v>144</v>
+        <v>216</v>
       </c>
       <c r="H28">
-        <v>134</v>
+        <v>215</v>
       </c>
       <c r="I28">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="J28">
-        <v>126</v>
+        <v>197</v>
       </c>
       <c r="K28">
-        <v>135</v>
+        <v>189</v>
+      </c>
+      <c r="L28">
+        <v>167</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ELFSM</t>
+          <t>EMR</t>
         </is>
       </c>
       <c r="B29">
-        <v>213</v>
+        <v>650</v>
       </c>
       <c r="C29">
-        <v>227</v>
+        <v>670</v>
       </c>
       <c r="D29">
-        <v>230</v>
+        <v>675</v>
       </c>
       <c r="E29">
-        <v>228</v>
+        <v>664</v>
       </c>
       <c r="F29">
-        <v>221</v>
+        <v>660</v>
       </c>
       <c r="G29">
-        <v>216</v>
+        <v>649</v>
       </c>
       <c r="H29">
-        <v>215</v>
+        <v>638</v>
       </c>
       <c r="I29">
-        <v>193</v>
+        <v>617</v>
       </c>
       <c r="J29">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="K29">
-        <v>189</v>
+        <v>142</v>
+      </c>
+      <c r="L29">
+        <v>143</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>EMG</t>
+          <t>EMS</t>
         </is>
       </c>
       <c r="B30">
-        <v>498</v>
+        <v>3011</v>
       </c>
       <c r="C30">
-        <v>512</v>
+        <v>3140</v>
       </c>
       <c r="D30">
-        <v>513</v>
+        <v>3208</v>
       </c>
       <c r="E30">
-        <v>509</v>
+        <v>3198</v>
       </c>
       <c r="F30">
-        <v>508</v>
+        <v>3170</v>
       </c>
       <c r="G30">
-        <v>502</v>
+        <v>3046</v>
       </c>
       <c r="H30">
-        <v>488</v>
+        <v>3056</v>
       </c>
       <c r="I30">
-        <v>470</v>
+        <v>3043</v>
+      </c>
+      <c r="J30">
+        <v>3021</v>
+      </c>
+      <c r="K30">
+        <v>3039</v>
+      </c>
+      <c r="L30">
+        <v>3192</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>EMS</t>
+          <t>EMT</t>
         </is>
       </c>
       <c r="B31">
-        <v>3011</v>
+        <v>4250</v>
       </c>
       <c r="C31">
-        <v>3140</v>
+        <v>4659</v>
       </c>
       <c r="D31">
-        <v>3208</v>
+        <v>4861</v>
       </c>
       <c r="E31">
-        <v>3198</v>
+        <v>4908</v>
       </c>
       <c r="F31">
-        <v>3170</v>
+        <v>4858</v>
       </c>
       <c r="G31">
-        <v>3046</v>
+        <v>5007</v>
       </c>
       <c r="H31">
-        <v>3056</v>
+        <v>5116</v>
       </c>
       <c r="I31">
-        <v>3043</v>
+        <v>5186</v>
       </c>
       <c r="J31">
-        <v>3021</v>
+        <v>5347</v>
       </c>
       <c r="K31">
-        <v>3039</v>
+        <v>5448</v>
+      </c>
+      <c r="L31">
+        <v>6015</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>EMT</t>
+          <t>ENEL CE</t>
         </is>
       </c>
       <c r="B32">
-        <v>4250</v>
+        <v>6444</v>
       </c>
       <c r="C32">
-        <v>4659</v>
+        <v>6990</v>
       </c>
       <c r="D32">
-        <v>4861</v>
+        <v>7438</v>
       </c>
       <c r="E32">
-        <v>4908</v>
+        <v>7655</v>
       </c>
       <c r="F32">
-        <v>4858</v>
+        <v>7726</v>
       </c>
       <c r="G32">
-        <v>5007</v>
+        <v>10161</v>
       </c>
       <c r="H32">
-        <v>5116</v>
+        <v>8512</v>
       </c>
       <c r="I32">
-        <v>5186</v>
+        <v>9006</v>
       </c>
       <c r="J32">
-        <v>5347</v>
+        <v>10912</v>
       </c>
       <c r="K32">
-        <v>5448</v>
+        <v>9761</v>
+      </c>
+      <c r="L32">
+        <v>9141</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ENEL CE</t>
+          <t>ENEL RJ</t>
         </is>
       </c>
       <c r="B33">
-        <v>6444</v>
+        <v>5209</v>
       </c>
       <c r="C33">
-        <v>6990</v>
+        <v>5373</v>
       </c>
       <c r="D33">
-        <v>7438</v>
+        <v>5370</v>
       </c>
       <c r="E33">
-        <v>7655</v>
+        <v>6701</v>
       </c>
       <c r="F33">
-        <v>7726</v>
+        <v>6614</v>
       </c>
       <c r="G33">
-        <v>10161</v>
+        <v>4544</v>
       </c>
       <c r="H33">
-        <v>8512</v>
+        <v>4375</v>
       </c>
       <c r="I33">
-        <v>9006</v>
+        <v>4243</v>
       </c>
       <c r="J33">
-        <v>10912</v>
+        <v>4497</v>
       </c>
       <c r="K33">
-        <v>9761</v>
+        <v>5547</v>
+      </c>
+      <c r="L33">
+        <v>4358</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ENEL RJ</t>
+          <t>ENEL SP</t>
         </is>
       </c>
       <c r="B34">
-        <v>5209</v>
+        <v>12952</v>
       </c>
       <c r="C34">
-        <v>5373</v>
+        <v>13077</v>
       </c>
       <c r="D34">
-        <v>5370</v>
+        <v>13038</v>
       </c>
       <c r="E34">
-        <v>6701</v>
+        <v>12634</v>
       </c>
       <c r="F34">
-        <v>6614</v>
+        <v>12437</v>
       </c>
       <c r="G34">
-        <v>4544</v>
+        <v>12421</v>
       </c>
       <c r="H34">
-        <v>4375</v>
+        <v>12125</v>
       </c>
       <c r="I34">
-        <v>4243</v>
+        <v>11532</v>
       </c>
       <c r="J34">
-        <v>4497</v>
+        <v>11039</v>
       </c>
       <c r="K34">
-        <v>5547</v>
+        <v>10895</v>
+      </c>
+      <c r="L34">
+        <v>10167</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ENEL SP</t>
+          <t>EPB</t>
         </is>
       </c>
       <c r="B35">
-        <v>12952</v>
+        <v>1923</v>
       </c>
       <c r="C35">
-        <v>13077</v>
+        <v>2035</v>
       </c>
       <c r="D35">
-        <v>13038</v>
+        <v>2129</v>
       </c>
       <c r="E35">
-        <v>12634</v>
+        <v>2158</v>
       </c>
       <c r="F35">
-        <v>12437</v>
+        <v>2141</v>
       </c>
       <c r="G35">
-        <v>12421</v>
+        <v>2205</v>
       </c>
       <c r="H35">
-        <v>12125</v>
+        <v>2216</v>
       </c>
       <c r="I35">
-        <v>11532</v>
+        <v>2179</v>
       </c>
       <c r="J35">
-        <v>11039</v>
+        <v>2120</v>
       </c>
       <c r="K35">
-        <v>10895</v>
+        <v>2110</v>
+      </c>
+      <c r="L35">
+        <v>2419</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ENF</t>
+          <t>EQUATORIAL AL</t>
         </is>
       </c>
       <c r="B36">
-        <v>152</v>
+        <v>2150</v>
       </c>
       <c r="C36">
-        <v>158</v>
+        <v>2146</v>
       </c>
       <c r="D36">
-        <v>162</v>
+        <v>2172</v>
       </c>
       <c r="E36">
-        <v>155</v>
+        <v>2201</v>
       </c>
       <c r="F36">
-        <v>152</v>
+        <v>1907</v>
       </c>
       <c r="G36">
-        <v>147</v>
+        <v>2172</v>
       </c>
       <c r="H36">
-        <v>150</v>
+        <v>2086</v>
       </c>
       <c r="I36">
-        <v>147</v>
+        <v>2119</v>
       </c>
       <c r="J36">
-        <v>135</v>
+        <v>2113</v>
       </c>
       <c r="K36">
-        <v>142</v>
+        <v>2157</v>
+      </c>
+      <c r="L36">
+        <v>2154</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>EPB</t>
+          <t>EQUATORIAL GO</t>
         </is>
       </c>
       <c r="B37">
-        <v>1581</v>
+        <v>7904</v>
       </c>
       <c r="C37">
-        <v>1674</v>
+        <v>8154</v>
       </c>
       <c r="D37">
-        <v>1754</v>
+        <v>8366</v>
       </c>
       <c r="E37">
-        <v>1783</v>
+        <v>8519</v>
       </c>
       <c r="F37">
-        <v>1768</v>
+        <v>8490</v>
       </c>
       <c r="G37">
-        <v>1820</v>
+        <v>8531</v>
       </c>
       <c r="H37">
-        <v>1827</v>
+        <v>8266</v>
       </c>
       <c r="I37">
-        <v>1819</v>
+        <v>8108</v>
       </c>
       <c r="J37">
-        <v>1756</v>
+        <v>8065</v>
       </c>
       <c r="K37">
-        <v>1748</v>
+        <v>7950</v>
+      </c>
+      <c r="L37">
+        <v>8031</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>EQUATORIAL AL</t>
+          <t>EQUATORIAL MA</t>
         </is>
       </c>
       <c r="B38">
-        <v>2150</v>
+        <v>2250</v>
       </c>
       <c r="C38">
-        <v>2146</v>
+        <v>2363</v>
       </c>
       <c r="D38">
-        <v>2172</v>
+        <v>2461</v>
       </c>
       <c r="E38">
-        <v>2201</v>
+        <v>2673</v>
       </c>
       <c r="F38">
-        <v>1907</v>
+        <v>2815</v>
       </c>
       <c r="G38">
-        <v>2172</v>
+        <v>2879</v>
       </c>
       <c r="H38">
-        <v>2086</v>
+        <v>2955</v>
       </c>
       <c r="I38">
-        <v>2119</v>
+        <v>2941</v>
       </c>
       <c r="J38">
-        <v>2113</v>
+        <v>2838</v>
       </c>
       <c r="K38">
-        <v>2157</v>
+        <v>3001</v>
+      </c>
+      <c r="L38">
+        <v>3091</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>EQUATORIAL GO</t>
+          <t>EQUATORIAL PA</t>
         </is>
       </c>
       <c r="B39">
-        <v>7904</v>
+        <v>4061</v>
       </c>
       <c r="C39">
-        <v>8154</v>
+        <v>4112</v>
       </c>
       <c r="D39">
-        <v>8366</v>
+        <v>4308</v>
       </c>
       <c r="E39">
-        <v>8519</v>
+        <v>4582</v>
       </c>
       <c r="F39">
-        <v>8490</v>
+        <v>4319</v>
       </c>
       <c r="G39">
-        <v>8531</v>
+        <v>4457</v>
       </c>
       <c r="H39">
-        <v>8266</v>
+        <v>4460</v>
       </c>
       <c r="I39">
-        <v>8108</v>
+        <v>4306</v>
       </c>
       <c r="J39">
-        <v>8065</v>
+        <v>4414</v>
       </c>
       <c r="K39">
-        <v>7950</v>
+        <v>4400</v>
+      </c>
+      <c r="L39">
+        <v>4388</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>EQUATORIAL MA</t>
+          <t>EQUATORIAL PI</t>
         </is>
       </c>
       <c r="B40">
-        <v>2250</v>
+        <v>1728</v>
       </c>
       <c r="C40">
-        <v>2363</v>
+        <v>1825</v>
       </c>
       <c r="D40">
-        <v>2461</v>
+        <v>1896</v>
       </c>
       <c r="E40">
-        <v>2673</v>
+        <v>1988</v>
       </c>
       <c r="F40">
-        <v>2815</v>
+        <v>2036</v>
       </c>
       <c r="G40">
-        <v>2879</v>
+        <v>2011</v>
       </c>
       <c r="H40">
-        <v>2955</v>
+        <v>2065</v>
       </c>
       <c r="I40">
-        <v>2941</v>
+        <v>1966</v>
       </c>
       <c r="J40">
-        <v>2838</v>
+        <v>1934</v>
       </c>
       <c r="K40">
-        <v>3001</v>
+        <v>1926</v>
+      </c>
+      <c r="L40">
+        <v>1943</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>EQUATORIAL PA</t>
+          <t>ERO</t>
         </is>
       </c>
       <c r="B41">
-        <v>4061</v>
+        <v>2039</v>
       </c>
       <c r="C41">
-        <v>4112</v>
+        <v>2121</v>
       </c>
       <c r="D41">
-        <v>4308</v>
+        <v>2205</v>
       </c>
       <c r="E41">
-        <v>4582</v>
+        <v>2228</v>
       </c>
       <c r="F41">
-        <v>4319</v>
+        <v>2197</v>
       </c>
       <c r="G41">
-        <v>4457</v>
+        <v>2175</v>
       </c>
       <c r="H41">
-        <v>4460</v>
+        <v>2184</v>
       </c>
       <c r="I41">
-        <v>4306</v>
+        <v>2183</v>
       </c>
       <c r="J41">
-        <v>4414</v>
+        <v>2207</v>
       </c>
       <c r="K41">
-        <v>4400</v>
+        <v>2219</v>
+      </c>
+      <c r="L41">
+        <v>2269</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>EQUATORIAL PI</t>
+          <t>ESE</t>
         </is>
       </c>
       <c r="B42">
-        <v>1728</v>
+        <v>1223</v>
       </c>
       <c r="C42">
-        <v>1825</v>
+        <v>1255</v>
       </c>
       <c r="D42">
-        <v>1896</v>
+        <v>1267</v>
       </c>
       <c r="E42">
-        <v>1988</v>
+        <v>1271</v>
       </c>
       <c r="F42">
-        <v>2036</v>
+        <v>1274</v>
       </c>
       <c r="G42">
-        <v>2011</v>
+        <v>1288</v>
       </c>
       <c r="H42">
-        <v>2065</v>
+        <v>1261</v>
       </c>
       <c r="I42">
-        <v>1966</v>
+        <v>1232</v>
       </c>
       <c r="J42">
-        <v>1934</v>
+        <v>1210</v>
       </c>
       <c r="K42">
-        <v>1926</v>
+        <v>1172</v>
+      </c>
+      <c r="L42">
+        <v>1143</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ERO</t>
+          <t>ESS</t>
         </is>
       </c>
       <c r="B43">
-        <v>2039</v>
+        <v>1869</v>
       </c>
       <c r="C43">
-        <v>2121</v>
+        <v>1937</v>
       </c>
       <c r="D43">
-        <v>2205</v>
+        <v>1979</v>
       </c>
       <c r="E43">
-        <v>2228</v>
+        <v>1980</v>
       </c>
       <c r="F43">
-        <v>2197</v>
+        <v>1949</v>
       </c>
       <c r="G43">
-        <v>2175</v>
+        <v>1972</v>
       </c>
       <c r="H43">
-        <v>2184</v>
+        <v>1986</v>
       </c>
       <c r="I43">
-        <v>2183</v>
+        <v>1959</v>
       </c>
       <c r="J43">
-        <v>2207</v>
+        <v>1937</v>
       </c>
       <c r="K43">
-        <v>2219</v>
+        <v>1957</v>
+      </c>
+      <c r="L43">
+        <v>1939</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ESE</t>
+          <t>ETO</t>
         </is>
       </c>
       <c r="B44">
-        <v>1223</v>
+        <v>1092</v>
       </c>
       <c r="C44">
-        <v>1255</v>
+        <v>1147</v>
       </c>
       <c r="D44">
+        <v>1185</v>
+      </c>
+      <c r="E44">
+        <v>1205</v>
+      </c>
+      <c r="F44">
+        <v>1248</v>
+      </c>
+      <c r="G44">
+        <v>1242</v>
+      </c>
+      <c r="H44">
         <v>1267</v>
       </c>
-      <c r="E44">
-        <v>1271</v>
-      </c>
-      <c r="F44">
-        <v>1274</v>
-      </c>
-      <c r="G44">
-        <v>1288</v>
-      </c>
-      <c r="H44">
-        <v>1261</v>
-      </c>
       <c r="I44">
-        <v>1232</v>
+        <v>1257</v>
       </c>
       <c r="J44">
-        <v>1210</v>
+        <v>1242</v>
       </c>
       <c r="K44">
-        <v>1172</v>
+        <v>1268</v>
+      </c>
+      <c r="L44">
+        <v>1231</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ESS</t>
+          <t>HIDROPAN</t>
         </is>
       </c>
       <c r="B45">
-        <v>1869</v>
+        <v>72</v>
       </c>
       <c r="C45">
-        <v>1937</v>
+        <v>75</v>
       </c>
       <c r="D45">
-        <v>1979</v>
+        <v>77</v>
       </c>
       <c r="E45">
-        <v>1980</v>
+        <v>78</v>
       </c>
       <c r="F45">
-        <v>1949</v>
+        <v>78</v>
       </c>
       <c r="G45">
-        <v>1972</v>
+        <v>78</v>
       </c>
       <c r="H45">
-        <v>1986</v>
+        <v>79</v>
       </c>
       <c r="I45">
-        <v>1959</v>
+        <v>80</v>
       </c>
       <c r="J45">
-        <v>1937</v>
+        <v>76</v>
       </c>
       <c r="K45">
-        <v>1957</v>
+        <v>74</v>
+      </c>
+      <c r="L45">
+        <v>78</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ETO</t>
+          <t>LIGHT</t>
         </is>
       </c>
       <c r="B46">
-        <v>1092</v>
+        <v>6950</v>
       </c>
       <c r="C46">
-        <v>1147</v>
+        <v>7025</v>
       </c>
       <c r="D46">
-        <v>1185</v>
+        <v>6809</v>
       </c>
       <c r="E46">
-        <v>1205</v>
+        <v>6215</v>
       </c>
       <c r="F46">
-        <v>1248</v>
+        <v>6143</v>
       </c>
       <c r="G46">
-        <v>1242</v>
+        <v>5737</v>
       </c>
       <c r="H46">
-        <v>1267</v>
+        <v>5537</v>
       </c>
       <c r="I46">
-        <v>1257</v>
+        <v>3815</v>
       </c>
       <c r="J46">
-        <v>1242</v>
+        <v>4137</v>
       </c>
       <c r="K46">
-        <v>1268</v>
+        <v>4646</v>
+      </c>
+      <c r="L46">
+        <v>4141</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>HIDROPAN</t>
+          <t>MUXENERGIA</t>
         </is>
       </c>
       <c r="B47">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="C47">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="D47">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="E47">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="F47">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="G47">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="H47">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="I47">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="J47">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="K47">
-        <v>74</v>
+        <v>27</v>
+      </c>
+      <c r="L47">
+        <v>25</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>LIGHT</t>
+          <t>OUTRA</t>
         </is>
       </c>
       <c r="B48">
-        <v>6950</v>
+        <v>1692</v>
       </c>
       <c r="C48">
-        <v>7025</v>
+        <v>1832</v>
       </c>
       <c r="D48">
-        <v>6809</v>
+        <v>1939</v>
       </c>
       <c r="E48">
-        <v>6215</v>
+        <v>2056</v>
       </c>
       <c r="F48">
-        <v>6143</v>
+        <v>2153</v>
       </c>
       <c r="G48">
-        <v>5737</v>
+        <v>2371</v>
       </c>
       <c r="H48">
-        <v>5537</v>
+        <v>2667</v>
       </c>
       <c r="I48">
-        <v>3815</v>
+        <v>2777</v>
       </c>
       <c r="J48">
-        <v>4137</v>
+        <v>2849</v>
       </c>
       <c r="K48">
-        <v>4646</v>
+        <v>2967</v>
+      </c>
+      <c r="L48">
+        <v>3020</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>MUXENERGIA</t>
+          <t>PACTO</t>
         </is>
       </c>
       <c r="B49">
+        <v>23</v>
+      </c>
+      <c r="C49">
         <v>26</v>
       </c>
-      <c r="C49">
+      <c r="D49">
+        <v>26</v>
+      </c>
+      <c r="E49">
+        <v>24</v>
+      </c>
+      <c r="F49">
         <v>27</v>
       </c>
-      <c r="D49">
+      <c r="G49">
         <v>27</v>
       </c>
-      <c r="E49">
-        <v>27</v>
-      </c>
-      <c r="F49">
-        <v>28</v>
-      </c>
-      <c r="G49">
-        <v>28</v>
-      </c>
       <c r="H49">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I49">
         <v>28</v>
       </c>
       <c r="J49">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="K49">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="L49">
+        <v>25</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>OUTRA</t>
+          <t>RGE</t>
         </is>
       </c>
       <c r="B50">
-        <v>1692</v>
+        <v>12282</v>
       </c>
       <c r="C50">
-        <v>1832</v>
+        <v>12544</v>
       </c>
       <c r="D50">
-        <v>1939</v>
+        <v>12682</v>
       </c>
       <c r="E50">
-        <v>2056</v>
+        <v>12415</v>
       </c>
       <c r="F50">
-        <v>2153</v>
+        <v>12108</v>
       </c>
       <c r="G50">
-        <v>2371</v>
+        <v>11924</v>
       </c>
       <c r="H50">
-        <v>2667</v>
+        <v>11431</v>
       </c>
       <c r="I50">
-        <v>2777</v>
+        <v>12136</v>
       </c>
       <c r="J50">
-        <v>2849</v>
+        <v>10995</v>
       </c>
       <c r="K50">
-        <v>2967</v>
+        <v>11259</v>
+      </c>
+      <c r="L50">
+        <v>9737</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>PACTO</t>
+          <t>RORAIMA</t>
         </is>
       </c>
       <c r="B51">
-        <v>23</v>
+        <v>543</v>
       </c>
       <c r="C51">
-        <v>26</v>
+        <v>600</v>
       </c>
       <c r="D51">
-        <v>26</v>
+        <v>630</v>
       </c>
       <c r="E51">
-        <v>24</v>
+        <v>630</v>
       </c>
       <c r="F51">
-        <v>27</v>
+        <v>656</v>
       </c>
       <c r="G51">
-        <v>27</v>
+        <v>678</v>
       </c>
       <c r="H51">
-        <v>26</v>
+        <v>751</v>
       </c>
       <c r="I51">
-        <v>28</v>
+        <v>764</v>
       </c>
       <c r="J51">
-        <v>22</v>
+        <v>791</v>
       </c>
       <c r="K51">
-        <v>22</v>
+        <v>820</v>
+      </c>
+      <c r="L51">
+        <v>867</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>RGE</t>
+          <t>SULGIPE</t>
         </is>
       </c>
       <c r="B52">
-        <v>12282</v>
+        <v>127</v>
       </c>
       <c r="C52">
-        <v>12544</v>
+        <v>140</v>
       </c>
       <c r="D52">
-        <v>12682</v>
+        <v>141</v>
       </c>
       <c r="E52">
-        <v>12415</v>
+        <v>141</v>
       </c>
       <c r="F52">
-        <v>12108</v>
+        <v>142</v>
       </c>
       <c r="G52">
-        <v>11924</v>
+        <v>135</v>
       </c>
       <c r="H52">
-        <v>11431</v>
+        <v>131</v>
       </c>
       <c r="I52">
-        <v>12136</v>
+        <v>30</v>
       </c>
       <c r="J52">
-        <v>10995</v>
+        <v>110</v>
       </c>
       <c r="K52">
-        <v>11259</v>
+        <v>111</v>
+      </c>
+      <c r="L52">
+        <v>97</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>RORAIMA</t>
+          <t>UHENPAL</t>
         </is>
       </c>
       <c r="B53">
-        <v>543</v>
+        <v>41</v>
       </c>
       <c r="C53">
-        <v>600</v>
+        <v>43</v>
       </c>
       <c r="D53">
-        <v>630</v>
+        <v>46</v>
       </c>
       <c r="E53">
-        <v>630</v>
+        <v>46</v>
       </c>
       <c r="F53">
-        <v>656</v>
+        <v>40</v>
       </c>
       <c r="G53">
-        <v>678</v>
+        <v>45</v>
       </c>
       <c r="H53">
-        <v>751</v>
+        <v>49</v>
       </c>
       <c r="I53">
-        <v>764</v>
+        <v>49</v>
       </c>
       <c r="J53">
-        <v>791</v>
+        <v>48</v>
       </c>
       <c r="K53">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>SULGIPE</t>
-        </is>
-      </c>
-      <c r="B54">
-        <v>127</v>
-      </c>
-      <c r="C54">
-        <v>140</v>
-      </c>
-      <c r="D54">
-        <v>141</v>
-      </c>
-      <c r="E54">
-        <v>141</v>
-      </c>
-      <c r="F54">
-        <v>142</v>
-      </c>
-      <c r="G54">
-        <v>135</v>
-      </c>
-      <c r="H54">
-        <v>131</v>
-      </c>
-      <c r="I54">
-        <v>30</v>
-      </c>
-      <c r="J54">
-        <v>110</v>
-      </c>
-      <c r="K54">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>UHENPAL</t>
-        </is>
-      </c>
-      <c r="B55">
-        <v>41</v>
-      </c>
-      <c r="C55">
-        <v>43</v>
-      </c>
-      <c r="D55">
+        <v>49</v>
+      </c>
+      <c r="L53">
         <v>46</v>
-      </c>
-      <c r="E55">
-        <v>46</v>
-      </c>
-      <c r="F55">
-        <v>40</v>
-      </c>
-      <c r="G55">
-        <v>45</v>
-      </c>
-      <c r="H55">
-        <v>49</v>
-      </c>
-      <c r="I55">
-        <v>49</v>
-      </c>
-      <c r="J55">
-        <v>48</v>
-      </c>
-      <c r="K55">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>